<commit_message>
Updated Expenses sheet for 1) Bill Links added 2) Bill for CAN Analyzer
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{515B7651-9070-4DE8-8AF2-A577AC4282AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7134B0-B42C-4C59-A334-9B17C07FF392}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98B0F2DB-BDC1-4363-BB7A-E62F248CBCB3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Sr. No</t>
   </si>
@@ -82,12 +82,51 @@
 1 burgstrip male
 1K pot</t>
   </si>
+  <si>
+    <t>Bill_1</t>
+  </si>
+  <si>
+    <t>Bill_2</t>
+  </si>
+  <si>
+    <t>Bill_3</t>
+  </si>
+  <si>
+    <t>Bill_4</t>
+  </si>
+  <si>
+    <t>Bill_5</t>
+  </si>
+  <si>
+    <t>Petrol Expenses</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total Petrol + Expenses</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>CAN Analyzer</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Battery Pack and BMS</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,16 +142,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -135,20 +188,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -461,148 +545,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE97DF2-F2E7-40E3-BC6A-817177CF2128}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="H1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>44088</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>295</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="G2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1">
+        <v>100</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1">
+        <f>E2+E3+E4+E6</f>
+        <v>2363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>44169</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>337</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1">
+        <v>100</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="1">
+        <f>E5+E7</f>
+        <v>3771</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>44209</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1302</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>44216</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>744</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>44218</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>429</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3027</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>18750</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <f>SUM(E2:E8)</f>
+        <v>6134</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <f>SUM(H2:H8)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <f>E9+H9</f>
+        <v>6634</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>5000</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="1">
+        <f>E10-E11</f>
+        <v>1634</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{4CA7FF62-E980-4B6B-BA67-80812B9D19EF}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{4BC87973-26E5-4D77-9AAB-57C0CC92B14E}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{F3429F02-5C52-40D2-A235-5194401B18AE}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{F4676592-0DFC-487D-AD72-3B7956F40317}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{7CA6C4E7-D875-4DBD-8F3A-BC5EDF64B512}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Expenses Details with new sheet added with individual expenses and few updates
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7134B0-B42C-4C59-A334-9B17C07FF392}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C0448B-442E-4F29-B79A-82626A50A960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98B0F2DB-BDC1-4363-BB7A-E62F248CBCB3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Expenses" sheetId="1" r:id="rId1"/>
+    <sheet name="Internal" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Sr. No</t>
   </si>
@@ -119,7 +120,40 @@
     <t>Battery Pack and BMS</t>
   </si>
   <si>
-    <t>Person</t>
+    <t>Soby</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Total Expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount </t>
+  </si>
+  <si>
+    <t>Sr No.</t>
+  </si>
+  <si>
+    <t>From Individual</t>
+  </si>
+  <si>
+    <t>To Idividual</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Paid as a kick start amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paid Procurement Charges for initial components and testing </t>
+  </si>
+  <si>
+    <t>Paid as a share of Engineering Cost</t>
   </si>
 </sst>
 </file>
@@ -215,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -230,6 +264,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,15 +583,16 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -585,10 +621,10 @@
         <v>19</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -654,7 +690,7 @@
       </c>
       <c r="M3" s="1">
         <f>E5+E7</f>
-        <v>3771</v>
+        <v>744</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -747,10 +783,10 @@
         <v>6</v>
       </c>
       <c r="E7" s="1">
-        <v>3027</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="1">
@@ -771,15 +807,17 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4"/>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
       <c r="I8" s="8">
-        <v>18750</v>
+        <v>29653</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -792,7 +830,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1">
         <f>SUM(E2:E8)</f>
-        <v>6134</v>
+        <v>3107</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -810,7 +848,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1">
         <f>E9+H9</f>
-        <v>6634</v>
+        <v>3607</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -831,8 +869,8 @@
         <v>24</v>
       </c>
       <c r="H11" s="1">
-        <f>E10-E11</f>
-        <v>1634</v>
+        <f>E11-E10</f>
+        <v>1393</v>
       </c>
     </row>
   </sheetData>
@@ -842,8 +880,253 @@
     <hyperlink ref="G4" r:id="rId3" xr:uid="{F3429F02-5C52-40D2-A235-5194401B18AE}"/>
     <hyperlink ref="G5" r:id="rId4" xr:uid="{F4676592-0DFC-487D-AD72-3B7956F40317}"/>
     <hyperlink ref="G6" r:id="rId5" xr:uid="{7CA6C4E7-D875-4DBD-8F3A-BC5EDF64B512}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{CE85920A-7FC1-4D83-8E59-46FD71301B7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A81190-15D4-4763-BD77-DD0BBFBB015B}">
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20000</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1] Added Requirement sign-off document 2] Updated Requirement document to revision 0.0.3 3] Updated planning sheet with status today 4] Updated Expenses sheet with addition of one more sheet to track record
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C0448B-442E-4F29-B79A-82626A50A960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC85483-8583-4F2C-9F31-4BB17C4F3BAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{98B0F2DB-BDC1-4363-BB7A-E62F248CBCB3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{98B0F2DB-BDC1-4363-BB7A-E62F248CBCB3}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Sr. No</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Paid as a share of Engineering Cost</t>
+  </si>
+  <si>
+    <t>Sobby</t>
   </si>
 </sst>
 </file>
@@ -582,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE97DF2-F2E7-40E3-BC6A-817177CF2128}">
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,12 +894,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A81190-15D4-4763-BD77-DD0BBFBB015B}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -928,12 +934,14 @@
         <v>20000</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="2">
+        <v>44214</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
@@ -946,12 +954,14 @@
         <v>5000</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="2">
+        <v>44214</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>36</v>
       </c>
@@ -969,7 +979,9 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="2">
+        <v>44217</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Adding Bill 11 to the bills Section
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Solutions\Parag_LiBaAS\Lithium-ion_battery_as_service.git\trunk\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FA7205-6ED3-4A1C-8234-0AE953E3A3D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
     <sheet name="Internal" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Sr. No</t>
   </si>
@@ -178,11 +179,14 @@
   <si>
     <t>Bill_10</t>
   </si>
+  <si>
+    <t>Burgstrips</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,23 +607,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -651,7 +655,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -684,7 +688,7 @@
         <v>9461</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -717,7 +721,7 @@
         <v>3178</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -743,7 +747,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -769,7 +773,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -795,7 +799,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -817,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -845,7 +849,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -867,7 +871,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -893,7 +897,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -919,19 +923,31 @@
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1">
+        <v>94</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1">
+        <v>100</v>
+      </c>
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -943,7 +959,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
@@ -952,16 +968,16 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1">
         <f>SUM(E2:E13)</f>
-        <v>12639</v>
+        <v>12733</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1">
         <f>SUM(H2:H13)</f>
-        <v>600</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="5" t="s">
@@ -970,13 +986,13 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1">
         <f>E14+H14</f>
-        <v>13239</v>
+        <v>13433</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
@@ -993,19 +1009,19 @@
       </c>
       <c r="H16" s="1">
         <f>E16-E15</f>
-        <v>1761</v>
+        <v>1567</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
@@ -1013,22 +1029,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1048,7 +1064,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1068,7 +1084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1088,7 +1104,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1108,7 +1124,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1128,7 +1144,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1148,7 +1164,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1156,7 +1172,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1164,7 +1180,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1172,7 +1188,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1180,7 +1196,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1188,7 +1204,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1196,7 +1212,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1204,7 +1220,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1212,7 +1228,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1220,7 +1236,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1228,7 +1244,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1236,7 +1252,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1244,7 +1260,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1252,7 +1268,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1260,7 +1276,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1268,7 +1284,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1276,7 +1292,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Updated sheet with new bill for burg strip
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FA7205-6ED3-4A1C-8234-0AE953E3A3D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9661C2-58FB-4330-88D1-AD0C3A9D854A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Sr. No</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Burgstrips</t>
+  </si>
+  <si>
+    <t>Bill_11</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +943,9 @@
       <c r="F12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="H12" s="1">
         <v>100</v>
       </c>
@@ -1022,9 +1027,10 @@
     <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G12" r:id="rId9" xr:uid="{506D8716-E8F4-4D20-B943-AE66D45CF0F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Expense Details with following Expenses: 1] Added Battery pack delivery Dunzo Bill - Akshay 2] Updated Battery pack charger and Bulbs for load box experiment - Akshay
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Solutions\Parag_LiBaAS\Lithium-ion_battery_as_service.git\trunk\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Another_copy\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3A1883-A891-4066-9127-C4B87B7D62CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
     <sheet name="Internal" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>Sr. No</t>
   </si>
@@ -205,11 +206,20 @@
   <si>
     <t>PCB assembly</t>
   </si>
+  <si>
+    <t>Battery pack delivery</t>
+  </si>
+  <si>
+    <t>Charger Delivery from SSK home (Petrol 50Rs) + 4 bulbs for load experiment (15W 15 Rs each)</t>
+  </si>
+  <si>
+    <t>Bill_15</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -630,23 +640,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -678,7 +688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -711,7 +721,7 @@
         <v>9461</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -744,7 +754,7 @@
         <v>5256</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -770,7 +780,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -796,7 +806,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -822,7 +832,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -844,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -872,7 +882,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -894,7 +904,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -920,7 +930,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -946,7 +956,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -972,7 +982,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -996,7 +1006,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1020,7 +1030,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1044,8 +1054,10 @@
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="3" t="s">
         <v>54</v>
@@ -1062,31 +1074,55 @@
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="4"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>44368</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1">
+        <v>15</v>
+      </c>
+      <c r="E17" s="1">
+        <v>93</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
+    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>44374</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="E18" s="1">
+        <v>110</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="G18" s="4"/>
       <c r="H18" s="1"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -1095,7 +1131,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1">
         <f>SUM(E2:E18)</f>
-        <v>17311</v>
+        <v>17514</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1104,7 +1140,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="5" t="s">
@@ -1113,13 +1149,13 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1">
         <f>E19+H19</f>
-        <v>18011</v>
+        <v>18214</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
@@ -1136,46 +1172,47 @@
       </c>
       <c r="H21" s="1">
         <f>E21-E20</f>
-        <v>-3011</v>
+        <v>-3214</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G11" r:id="rId8"/>
-    <hyperlink ref="G12" r:id="rId9"/>
-    <hyperlink ref="G13" r:id="rId10"/>
-    <hyperlink ref="G14" r:id="rId11"/>
-    <hyperlink ref="G15" r:id="rId12"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G17" r:id="rId13" xr:uid="{0B2C7D5E-3DFE-46C2-9757-6EE8F44298A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1195,7 +1232,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1215,7 +1252,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1235,7 +1272,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1255,7 +1292,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1275,7 +1312,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1295,7 +1332,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1303,7 +1340,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1311,7 +1348,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1319,7 +1356,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1327,7 +1364,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1335,7 +1372,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1343,7 +1380,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1351,7 +1388,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1359,7 +1396,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1367,7 +1404,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1375,7 +1412,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1383,7 +1420,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1391,7 +1428,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1399,7 +1436,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1407,7 +1444,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1415,7 +1452,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1423,7 +1460,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Added 2 more bills 1] Bill_16 and 2] Bill_17
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Another_copy\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3A1883-A891-4066-9127-C4B87B7D62CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE311852-B9A6-4BD6-93C5-1A8DDC9A3C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
   <si>
     <t>Sr. No</t>
   </si>
@@ -214,6 +214,15 @@
   </si>
   <si>
     <t>Bill_15</t>
+  </si>
+  <si>
+    <t>Rajiv Electronics Bill</t>
+  </si>
+  <si>
+    <t>Bus Ticket Bill and Auto travel</t>
+  </si>
+  <si>
+    <t>(Auto500)</t>
   </si>
 </sst>
 </file>
@@ -641,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +661,7 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1123,56 +1133,108 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1"/>
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>44389</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="1">
+        <v>16</v>
+      </c>
       <c r="E19" s="1">
-        <f>SUM(E2:E18)</f>
-        <v>17514</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1">
-        <f>SUM(H2:H18)</f>
-        <v>700</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>1105</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="9"/>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44390</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="1">
+        <v>17</v>
+      </c>
       <c r="E20" s="1">
-        <f>E19+H19</f>
-        <v>18214</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+        <v>2205</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="1">
+        <v>500</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1">
+        <f>SUM(E2:E19)</f>
+        <v>18619</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1">
+        <f>SUM(H2:H18)</f>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1">
+        <f>E21+H21</f>
+        <v>19319</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1">
         <f>Internal!B3+Internal!B6</f>
         <v>15000</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="1">
-        <f>E21-E20</f>
-        <v>-3214</v>
+      <c r="H23" s="1">
+        <f>E23-E22</f>
+        <v>-4319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Expenses Sheet with 1] Bill_16 and 2] Bill_17
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Another_copy\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE311852-B9A6-4BD6-93C5-1A8DDC9A3C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0428722D-AA16-45CC-BA62-89030989486B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
   <si>
     <t>Sr. No</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>(Auto500)</t>
+  </si>
+  <si>
+    <t>Bill_16</t>
+  </si>
+  <si>
+    <t>Bill_17</t>
   </si>
 </sst>
 </file>
@@ -652,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,7 +1157,9 @@
       <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="4"/>
+      <c r="G19" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="11"/>
       <c r="J19" s="9"/>
@@ -1175,7 +1183,9 @@
       <c r="F20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="4"/>
+      <c r="G20" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="H20" s="1">
         <v>500</v>
       </c>
@@ -1252,9 +1262,11 @@
     <hyperlink ref="G14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="G15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="G17" r:id="rId13" xr:uid="{0B2C7D5E-3DFE-46C2-9757-6EE8F44298A6}"/>
+    <hyperlink ref="G19" r:id="rId14" xr:uid="{9EC4F45C-8747-4523-A4AA-FEA54B891172}"/>
+    <hyperlink ref="G20" r:id="rId15" xr:uid="{3698E5D8-E362-4A37-A44D-99BB127336BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding bills for Expenses while procuring components for 1] load box 2] Heat sink 3] others
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Another_copy\Lithium-ion_battery_as_service\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Solutions\Parag_LiBaAS\Git_checkout\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0428722D-AA16-45CC-BA62-89030989486B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
     <sheet name="Internal" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
   <si>
     <t>Sr. No</t>
   </si>
@@ -230,11 +229,65 @@
   <si>
     <t>Bill_17</t>
   </si>
+  <si>
+    <t>relays</t>
+  </si>
+  <si>
+    <t>hardware tools</t>
+  </si>
+  <si>
+    <t>Bill_18</t>
+  </si>
+  <si>
+    <t>Bill_19</t>
+  </si>
+  <si>
+    <t>Bill_20</t>
+  </si>
+  <si>
+    <t>cab</t>
+  </si>
+  <si>
+    <t>Bill_21</t>
+  </si>
+  <si>
+    <t>Bill_22</t>
+  </si>
+  <si>
+    <t>Bill_23</t>
+  </si>
+  <si>
+    <t>Bill_24</t>
+  </si>
+  <si>
+    <t>Bill_25</t>
+  </si>
+  <si>
+    <t>acrylic box</t>
+  </si>
+  <si>
+    <t>Bill_26</t>
+  </si>
+  <si>
+    <t>Bill_27</t>
+  </si>
+  <si>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>Bill_28</t>
+  </si>
+  <si>
+    <t>hardware components</t>
+  </si>
+  <si>
+    <t>Bill_29</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -655,24 +708,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -704,7 +757,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -737,7 +790,7 @@
         <v>9461</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -770,7 +823,7 @@
         <v>5256</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -796,7 +849,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -822,7 +875,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -848,7 +901,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -870,7 +923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -898,7 +951,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -920,7 +973,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -946,7 +999,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -972,7 +1025,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -998,7 +1051,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1022,7 +1075,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1046,7 +1099,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1070,223 +1123,547 @@
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2">
+        <v>44368</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <v>2500</v>
+        <v>93</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="4"/>
+        <v>8</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>57</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>44368</v>
+        <v>44374</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="1">
-        <v>15</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="1">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="G17" s="4"/>
       <c r="H17" s="1"/>
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>44374</v>
+        <v>44389</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="D18" s="1">
+        <v>16</v>
+      </c>
       <c r="E18" s="1">
-        <v>110</v>
+        <v>1105</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="1">
-        <v>1105</v>
+        <v>2205</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="H19" s="1">
+        <v>500</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>60</v>
+      </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>44375</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1">
+        <v>18</v>
+      </c>
+      <c r="E20" s="1">
+        <f>700+649+1645</f>
+        <v>2994</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44384</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
-        <v>44390</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D20" s="1">
-        <v>17</v>
-      </c>
-      <c r="E20" s="1">
-        <v>2205</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E21" s="1">
+        <v>550</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>44323</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="1">
+        <v>20</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" s="1"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="9"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44392</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="1">
+        <v>21</v>
+      </c>
+      <c r="E23" s="1">
+        <v>282</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="1">
-        <v>500</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+      <c r="G23" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>44412</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="1">
+        <v>22</v>
+      </c>
+      <c r="E24" s="1">
+        <v>246</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="1"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="9"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2">
+        <v>44412</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="1">
+        <v>23</v>
+      </c>
+      <c r="E25" s="1">
+        <v>266</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="9"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>44392</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="1">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1">
+        <v>336</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="9"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>44392</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="1">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1">
+        <v>384</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="9"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>44412</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="1">
+        <v>26</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1800</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="1"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="9"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>44392</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D29" s="1">
+        <v>27</v>
+      </c>
+      <c r="E29" s="1">
+        <v>175</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H29" s="1"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>44392</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="1">
+        <v>28</v>
+      </c>
+      <c r="E30" s="1">
+        <v>70</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="1"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="9"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44392</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="1">
+        <v>29</v>
+      </c>
+      <c r="E31" s="1">
+        <v>375</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H31" s="1"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="9"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="9"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1">
-        <f>SUM(E2:E19)</f>
-        <v>18619</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1">
-        <f>SUM(H2:H18)</f>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1">
+        <f>SUM(E2:E33)</f>
+        <v>28302</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1">
+        <f>SUM(H2:H17)</f>
         <v>700</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="5" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1">
-        <f>E21+H21</f>
-        <v>19319</v>
-      </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1">
+        <f>E34+H34</f>
+        <v>29002</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1">
         <f>Internal!B3+Internal!B6</f>
         <v>15000</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="1">
-        <f>E23-E22</f>
-        <v>-4319</v>
+      <c r="H36" s="1">
+        <f>E36-E35</f>
+        <v>-14002</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="G14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="G17" r:id="rId13" xr:uid="{0B2C7D5E-3DFE-46C2-9757-6EE8F44298A6}"/>
-    <hyperlink ref="G19" r:id="rId14" xr:uid="{9EC4F45C-8747-4523-A4AA-FEA54B891172}"/>
-    <hyperlink ref="G20" r:id="rId15" xr:uid="{3698E5D8-E362-4A37-A44D-99BB127336BE}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G4" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="G8" r:id="rId6"/>
+    <hyperlink ref="G10" r:id="rId7"/>
+    <hyperlink ref="G11" r:id="rId8"/>
+    <hyperlink ref="G12" r:id="rId9"/>
+    <hyperlink ref="G13" r:id="rId10"/>
+    <hyperlink ref="G14" r:id="rId11"/>
+    <hyperlink ref="G15" r:id="rId12"/>
+    <hyperlink ref="G16" r:id="rId13"/>
+    <hyperlink ref="G18" r:id="rId14"/>
+    <hyperlink ref="G19" r:id="rId15"/>
+    <hyperlink ref="G20" r:id="rId16"/>
+    <hyperlink ref="G21" r:id="rId17"/>
+    <hyperlink ref="G22" r:id="rId18"/>
+    <hyperlink ref="G23" r:id="rId19"/>
+    <hyperlink ref="G24" r:id="rId20"/>
+    <hyperlink ref="G25" r:id="rId21"/>
+    <hyperlink ref="G26" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1306,7 +1683,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1326,7 +1703,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1346,7 +1723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1366,7 +1743,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1386,7 +1763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1406,7 +1783,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1414,7 +1791,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1422,7 +1799,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1430,7 +1807,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1438,7 +1815,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1446,7 +1823,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1454,7 +1831,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1462,7 +1839,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1470,7 +1847,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1478,7 +1855,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1486,7 +1863,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1494,7 +1871,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1502,7 +1879,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1510,7 +1887,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1518,7 +1895,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1526,7 +1903,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1534,7 +1911,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
updated hyperlinks for all bills
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1641,9 +1641,14 @@
     <hyperlink ref="G24" r:id="rId20"/>
     <hyperlink ref="G25" r:id="rId21"/>
     <hyperlink ref="G26" r:id="rId22"/>
+    <hyperlink ref="G27" r:id="rId23"/>
+    <hyperlink ref="G28" r:id="rId24"/>
+    <hyperlink ref="G29" r:id="rId25"/>
+    <hyperlink ref="G30" r:id="rId26"/>
+    <hyperlink ref="G31" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated expenses which to be shared with sobby
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -977,7 +977,9 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>44249</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
@@ -1003,7 +1005,9 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>44254</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1029,7 +1033,9 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>44288</v>
+      </c>
       <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
@@ -1055,7 +1061,9 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>44312</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>48</v>
       </c>
@@ -1079,7 +1087,9 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <v>44327</v>
+      </c>
       <c r="C14" s="3" t="s">
         <v>50</v>
       </c>
@@ -1103,7 +1113,9 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>44281</v>
+      </c>
       <c r="C15" s="3" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Updated Expense Sheet with the bill of 500 Rs for shipment of Load Box Paid by Akshay Godase
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Solutions\Parag_LiBaAS\Git_checkout\Lithium-ion_battery_as_service\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77295747-2C88-4449-93AE-1118091D2BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses" sheetId="1" r:id="rId1"/>
     <sheet name="Internal" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="85">
   <si>
     <t>Sr. No</t>
   </si>
@@ -289,11 +290,17 @@
   <si>
     <t>Bill_30</t>
   </si>
+  <si>
+    <t>Courier Load Box</t>
+  </si>
+  <si>
+    <t>Bill_31</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -714,24 +721,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -763,7 +770,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -796,7 +803,7 @@
         <v>14245</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -829,7 +836,7 @@
         <v>16457</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -855,7 +862,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -881,7 +888,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -907,7 +914,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -929,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -957,7 +964,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -979,7 +986,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1007,7 +1014,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1035,7 +1042,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1063,7 +1070,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1089,7 +1096,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1115,7 +1122,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1141,7 +1148,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -1167,7 +1174,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -1189,7 +1196,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -1215,7 +1222,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -1245,7 +1252,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1272,7 +1279,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1298,7 +1305,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1324,7 +1331,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -1350,7 +1357,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -1376,7 +1383,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1402,7 +1409,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1428,7 +1435,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1454,7 +1461,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -1480,7 +1487,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -1506,7 +1513,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -1532,7 +1539,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -1558,7 +1565,7 @@
       <c r="I31" s="11"/>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -1586,19 +1593,33 @@
       <c r="I32" s="11"/>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="4"/>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>33</v>
+      </c>
+      <c r="B33" s="2">
+        <v>44420</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="1">
+        <v>31</v>
+      </c>
+      <c r="E33" s="1">
+        <v>500</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="11"/>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -1607,7 +1628,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1">
         <f>SUM(E2:E33)</f>
-        <v>30702</v>
+        <v>31202</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -1616,7 +1637,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="5" t="s">
@@ -1625,13 +1646,13 @@
       <c r="D35" s="1"/>
       <c r="E35" s="1">
         <f>E34+H34</f>
-        <v>32002</v>
+        <v>32502</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -1648,62 +1669,63 @@
       </c>
       <c r="H36" s="1">
         <f>E36-E35</f>
-        <v>-17002</v>
+        <v>-17502</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G11" r:id="rId8"/>
-    <hyperlink ref="G12" r:id="rId9"/>
-    <hyperlink ref="G13" r:id="rId10"/>
-    <hyperlink ref="G14" r:id="rId11"/>
-    <hyperlink ref="G15" r:id="rId12"/>
-    <hyperlink ref="G16" r:id="rId13"/>
-    <hyperlink ref="G18" r:id="rId14"/>
-    <hyperlink ref="G19" r:id="rId15"/>
-    <hyperlink ref="G20" r:id="rId16"/>
-    <hyperlink ref="G21" r:id="rId17"/>
-    <hyperlink ref="G22" r:id="rId18"/>
-    <hyperlink ref="G23" r:id="rId19"/>
-    <hyperlink ref="G24" r:id="rId20"/>
-    <hyperlink ref="G25" r:id="rId21"/>
-    <hyperlink ref="G26" r:id="rId22"/>
-    <hyperlink ref="G27" r:id="rId23"/>
-    <hyperlink ref="G28" r:id="rId24"/>
-    <hyperlink ref="G29" r:id="rId25"/>
-    <hyperlink ref="G30" r:id="rId26"/>
-    <hyperlink ref="G31" r:id="rId27"/>
-    <hyperlink ref="G32" r:id="rId28" display="Bill_29"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G32" r:id="rId28" display="Bill_29" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G33" r:id="rId29" xr:uid="{894EA139-57D7-4E9E-95C3-03D82FE82A42}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -1723,7 +1745,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1743,7 +1765,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1763,7 +1785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1783,7 +1805,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1803,7 +1825,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1823,7 +1845,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1831,7 +1853,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1839,7 +1861,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1847,7 +1869,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1855,7 +1877,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1863,7 +1885,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1871,7 +1893,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1879,7 +1901,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1887,7 +1909,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1895,7 +1917,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1903,7 +1925,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1911,7 +1933,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1919,7 +1941,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1927,7 +1949,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1935,7 +1957,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1943,7 +1965,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1951,7 +1973,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Updated expense sheet: 1] Restructured sheet with new way 2] Updated link for Bill_32
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -1,32 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Solutions\Parag_LiBaAS\Git_checkout\Lithium-ion_battery_as_service\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E093ABDC-97CC-420B-8FCA-1AC9321A1D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses_proto1" sheetId="1" r:id="rId1"/>
     <sheet name="Expenses_proto2" sheetId="4" r:id="rId2"/>
     <sheet name="Internal" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
   <si>
     <t>Sr. No</t>
   </si>
@@ -305,11 +313,25 @@
   <si>
     <t>Paid the reimbursement for 1st proto (Akshay Share)</t>
   </si>
+  <si>
+    <t>Courier Battery pack to Nikhil</t>
+  </si>
+  <si>
+    <t>Bill_32</t>
+  </si>
+  <si>
+    <t>Paid by
+Parag</t>
+  </si>
+  <si>
+    <t>Paid by
+Akshay</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -399,7 +421,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -416,6 +438,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -730,24 +755,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -779,7 +804,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -812,7 +837,7 @@
         <v>14245</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -845,7 +870,7 @@
         <v>16457</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -871,7 +896,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -897,7 +922,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -923,7 +948,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -945,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -973,7 +998,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -995,7 +1020,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1023,7 +1048,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1051,7 +1076,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1079,7 +1104,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1105,7 +1130,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1131,7 +1156,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1157,7 +1182,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -1183,7 +1208,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -1205,7 +1230,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -1231,7 +1256,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -1261,7 +1286,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1288,7 +1313,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1314,7 +1339,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1340,7 +1365,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -1366,7 +1391,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -1392,7 +1417,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1418,7 +1443,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1444,7 +1469,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1470,7 +1495,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -1496,7 +1521,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -1522,7 +1547,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -1548,7 +1573,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -1574,7 +1599,7 @@
       <c r="I31" s="11"/>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -1602,13 +1627,13 @@
       <c r="I32" s="11"/>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="11"/>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -1626,7 +1651,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="5" t="s">
@@ -1641,7 +1666,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -1663,34 +1688,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-    <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G6" r:id="rId5"/>
-    <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G10" r:id="rId7"/>
-    <hyperlink ref="G11" r:id="rId8"/>
-    <hyperlink ref="G12" r:id="rId9"/>
-    <hyperlink ref="G13" r:id="rId10"/>
-    <hyperlink ref="G14" r:id="rId11"/>
-    <hyperlink ref="G15" r:id="rId12"/>
-    <hyperlink ref="G16" r:id="rId13"/>
-    <hyperlink ref="G18" r:id="rId14"/>
-    <hyperlink ref="G19" r:id="rId15"/>
-    <hyperlink ref="G20" r:id="rId16"/>
-    <hyperlink ref="G21" r:id="rId17"/>
-    <hyperlink ref="G22" r:id="rId18"/>
-    <hyperlink ref="G23" r:id="rId19"/>
-    <hyperlink ref="G24" r:id="rId20"/>
-    <hyperlink ref="G25" r:id="rId21"/>
-    <hyperlink ref="G26" r:id="rId22"/>
-    <hyperlink ref="G27" r:id="rId23"/>
-    <hyperlink ref="G28" r:id="rId24"/>
-    <hyperlink ref="G29" r:id="rId25"/>
-    <hyperlink ref="G30" r:id="rId26"/>
-    <hyperlink ref="G31" r:id="rId27"/>
-    <hyperlink ref="G32" r:id="rId28" display="Bill_29"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="G10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="G15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="G19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="G22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="G25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G32" r:id="rId28" display="Bill_29" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
@@ -1698,24 +1723,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1731,23 +1757,26 @@
       <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1763,41 +1792,59 @@
       <c r="E2" s="1">
         <v>500</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>500</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="M2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="L2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="1">
-        <f>E2</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N2" s="1">
+        <f>G34</f>
+        <v>636</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="1"/>
-      <c r="L3" s="1" t="s">
+      <c r="B3" s="2">
+        <v>44524</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="1">
+        <v>32</v>
+      </c>
+      <c r="E3" s="1">
+        <v>136</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>136</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="1">
-        <f>E5+E7+E11+E13+E14+E15+E20+E21+E22+E24+E25+E28+E30+E31+E32</f>
+      <c r="N3" s="1">
+        <f>F34</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1806,10 +1853,11 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1818,10 +1866,11 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G5" s="1"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1830,10 +1879,11 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1842,10 +1892,11 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G7" s="1"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1854,12 +1905,13 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1868,12 +1920,13 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G9" s="1"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1882,12 +1935,13 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G10" s="1"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1896,12 +1950,13 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G11" s="1"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1910,12 +1965,13 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1924,12 +1980,13 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G13" s="1"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1938,12 +1995,13 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1952,12 +2010,13 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G15" s="1"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -1966,12 +2025,13 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G16" s="1"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -1980,12 +2040,13 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G17" s="1"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -1994,12 +2055,13 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -2008,12 +2070,13 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G19" s="1"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -2022,12 +2085,13 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G20" s="1"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -2036,12 +2100,13 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G21" s="1"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -2050,12 +2115,13 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G22" s="1"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -2064,12 +2130,13 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G23" s="1"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -2078,12 +2145,13 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G24" s="1"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -2092,12 +2160,13 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G25" s="1"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -2106,12 +2175,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="9"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G26" s="1"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -2120,12 +2190,13 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="9"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G27" s="1"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -2134,12 +2205,13 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="9"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G28" s="1"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -2148,12 +2220,13 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="9"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G29" s="1"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -2162,12 +2235,13 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="9"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G30" s="1"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -2176,12 +2250,13 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="9"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G31" s="1"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -2190,12 +2265,13 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="9"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G32" s="1"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -2204,12 +2280,13 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="9"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G33" s="1"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -2218,16 +2295,23 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1">
         <f>SUM(E2:E33)</f>
-        <v>500</v>
-      </c>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1">
-        <f>SUM(H2:H33)</f>
+        <v>636</v>
+      </c>
+      <c r="F34" s="1">
+        <f>SUM(F2:F33)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G34" s="1">
+        <f>SUM(G2:G33)</f>
+        <v>636</v>
+      </c>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1">
+        <f>SUM(I2:I33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="5" t="s">
@@ -2235,14 +2319,15 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1">
-        <f>E34+H34</f>
-        <v>500</v>
+        <f>E34+I34</f>
+        <v>636</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -2251,40 +2336,42 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="1">
+      <c r="I36" s="1">
         <f>E36-E35</f>
-        <v>-500</v>
+        <v>-636</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{F050F6C5-D1B0-4B73-B897-114F30EFDAE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -2304,7 +2391,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2324,7 +2411,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2344,7 +2431,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2364,7 +2451,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2384,7 +2471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2404,7 +2491,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2424,7 +2511,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2444,7 +2531,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2464,7 +2551,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2472,7 +2559,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2480,7 +2567,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2488,7 +2575,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2496,7 +2583,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2504,7 +2591,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2512,7 +2599,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2520,7 +2607,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2528,7 +2615,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2536,7 +2623,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2544,7 +2631,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2552,7 +2639,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2560,7 +2647,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2568,7 +2655,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>

<commit_message>
Updated expense sheet for Bill 34 and 35
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Lithium-ion_battery_as_service\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Another_copy\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E093ABDC-97CC-420B-8FCA-1AC9321A1D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2C1011-D5F9-4949-B8F2-EAA3085960C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
   <si>
     <t>Sr. No</t>
   </si>
@@ -326,6 +326,35 @@
   <si>
     <t>Paid by
 Akshay</t>
+  </si>
+  <si>
+    <t>Bill_33</t>
+  </si>
+  <si>
+    <t>Equipments purchased before Date of Deployment</t>
+  </si>
+  <si>
+    <t>Petrol for Nashik Travel</t>
+  </si>
+  <si>
+    <t>Battery Repairing Cost</t>
+  </si>
+  <si>
+    <t>Bill_34</t>
+  </si>
+  <si>
+    <t>Bill_35</t>
+  </si>
+  <si>
+    <t>Bill_</t>
+  </si>
+  <si>
+    <t>Own
+Pocket</t>
+  </si>
+  <si>
+    <t>Through
+10K</t>
   </si>
 </sst>
 </file>
@@ -421,7 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -439,6 +468,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1724,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,13 +1767,13 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1767,16 +1799,19 @@
         <v>6</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1801,16 +1836,19 @@
       <c r="H2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="M2" s="1" t="s">
+      <c r="I2" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <f>G34</f>
         <v>636</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1835,55 +1873,109 @@
       <c r="H3" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="M3" s="1" t="s">
+      <c r="I3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="N3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <f>F34</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6790</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>44532</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="1">
+        <v>33</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2390</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2390</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>44533</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3400</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3400</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>44476</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" s="1">
+        <v>35</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1893,10 +1985,13 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1906,12 +2001,15 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1921,12 +2019,15 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1936,12 +2037,15 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1951,12 +2055,15 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1966,12 +2073,15 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1981,12 +2091,15 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1996,12 +2109,15 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2011,12 +2127,15 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H15" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -2026,12 +2145,15 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -2041,12 +2163,15 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -2056,12 +2181,15 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -2071,12 +2199,15 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -2086,12 +2217,15 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -2101,12 +2235,15 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -2116,12 +2253,15 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H22" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -2131,12 +2271,15 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -2146,12 +2289,15 @@
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -2161,12 +2307,15 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -2176,12 +2325,15 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="9"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -2191,12 +2343,15 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="9"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H27" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="9"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -2206,12 +2361,15 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="9"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H28" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="9"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -2221,12 +2379,15 @@
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="9"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H29" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="9"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -2236,12 +2397,15 @@
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="9"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="9"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -2251,12 +2415,15 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="9"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="9"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -2266,12 +2433,15 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="9"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="9"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -2281,12 +2451,15 @@
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="9"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="9"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -2295,23 +2468,24 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1">
         <f>SUM(E2:E33)</f>
-        <v>636</v>
+        <v>7426</v>
       </c>
       <c r="F34" s="1">
         <f>SUM(F2:F33)</f>
-        <v>0</v>
+        <v>6790</v>
       </c>
       <c r="G34" s="1">
         <f>SUM(G2:G33)</f>
         <v>636</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1">
-        <f>SUM(I2:I33)</f>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="1">
+        <f>SUM(J2:J33)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="5" t="s">
@@ -2319,39 +2493,44 @@
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1">
-        <f>E34+I34</f>
-        <v>636</v>
+        <f>E34+J34</f>
+        <v>7426</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <v>10000</v>
+      </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="1"/>
+      <c r="J36" s="1">
         <f>E36-E35</f>
-        <v>-636</v>
+        <v>2574</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{F050F6C5-D1B0-4B73-B897-114F30EFDAE6}"/>
+    <hyperlink ref="H4" r:id="rId3" xr:uid="{016011F2-5F85-4351-B16C-59DA699D1A8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Bill_34 and Bill_35 links updated in the expense sheet
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Another_copy\Lithium-ion_battery_as_service\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2C1011-D5F9-4949-B8F2-EAA3085960C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D549C5E-86CF-4A69-B90D-7773EC1550E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1759,7 +1759,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2528,9 +2528,11 @@
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="H3" r:id="rId2" xr:uid="{F050F6C5-D1B0-4B73-B897-114F30EFDAE6}"/>
     <hyperlink ref="H4" r:id="rId3" xr:uid="{016011F2-5F85-4351-B16C-59DA699D1A8C}"/>
+    <hyperlink ref="H5" r:id="rId4" xr:uid="{ED46AF62-4EAA-456D-BD6F-0B89970FC3D1}"/>
+    <hyperlink ref="H6" r:id="rId5" xr:uid="{5B403C4B-1793-4BA3-ABED-2AE1B975D035}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added updated Expenses Details with latest change
Added 2 expenses which we received from Soby
</commit_message>
<xml_diff>
--- a/Docs/Expenses Details.xlsx
+++ b/Docs/Expenses Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aksha\Documents\Akshay\Projects\Another_copy\Lithium-ion_battery_as_service\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxf73403\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D549C5E-86CF-4A69-B90D-7773EC1550E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A26C4A-466D-4C8C-B610-652FEF485E99}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expenses_proto1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="103">
   <si>
     <t>Sr. No</t>
   </si>
@@ -355,6 +357,12 @@
   <si>
     <t>Through
 10K</t>
+  </si>
+  <si>
+    <t>Paid Procurement Charges for 2nd components and PCB</t>
+  </si>
+  <si>
+    <t>Paid for 2nd milestone partial</t>
   </si>
 </sst>
 </file>
@@ -790,21 +798,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.81640625" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -836,7 +844,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -869,7 +877,7 @@
         <v>14245</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -902,7 +910,7 @@
         <v>16457</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -928,7 +936,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -954,7 +962,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -980,7 +988,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1002,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1030,7 +1038,7 @@
       </c>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1052,7 +1060,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1080,7 +1088,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1108,7 +1116,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1136,7 +1144,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1162,7 +1170,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1188,7 +1196,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1214,7 +1222,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -1240,7 +1248,7 @@
       <c r="I16" s="11"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -1262,7 +1270,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -1288,7 +1296,7 @@
       <c r="I18" s="11"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -1318,7 +1326,7 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -1345,7 +1353,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -1371,7 +1379,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -1397,7 +1405,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -1423,7 +1431,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -1449,7 +1457,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -1475,7 +1483,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -1501,7 +1509,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -1527,7 +1535,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -1553,7 +1561,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -1579,7 +1587,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -1605,7 +1613,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -1631,7 +1639,7 @@
       <c r="I31" s="11"/>
       <c r="J31" s="9"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -1659,13 +1667,13 @@
       <c r="I32" s="11"/>
       <c r="J32" s="9"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="11"/>
       <c r="J33" s="9"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -1683,7 +1691,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="5" t="s">
@@ -1698,7 +1706,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -1758,22 +1766,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1811,7 +1819,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1848,7 +1856,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1885,7 +1893,7 @@
         <v>6790</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1915,7 +1923,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1945,7 +1953,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1975,7 +1983,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1991,7 +1999,7 @@
       <c r="I7" s="4"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2009,7 +2017,7 @@
       <c r="K8" s="8"/>
       <c r="L8" s="9"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2027,7 +2035,7 @@
       <c r="K9" s="11"/>
       <c r="L9" s="9"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2045,7 +2053,7 @@
       <c r="K10" s="11"/>
       <c r="L10" s="9"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -2063,7 +2071,7 @@
       <c r="K11" s="11"/>
       <c r="L11" s="9"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -2081,7 +2089,7 @@
       <c r="K12" s="11"/>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2099,7 +2107,7 @@
       <c r="K13" s="11"/>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2117,7 +2125,7 @@
       <c r="K14" s="11"/>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2135,7 +2143,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>16</v>
       </c>
@@ -2153,7 +2161,7 @@
       <c r="K16" s="11"/>
       <c r="L16" s="9"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>17</v>
       </c>
@@ -2171,7 +2179,7 @@
       <c r="K17" s="11"/>
       <c r="L17" s="9"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>18</v>
       </c>
@@ -2189,7 +2197,7 @@
       <c r="K18" s="11"/>
       <c r="L18" s="9"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>19</v>
       </c>
@@ -2207,7 +2215,7 @@
       <c r="K19" s="11"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>20</v>
       </c>
@@ -2225,7 +2233,7 @@
       <c r="K20" s="11"/>
       <c r="L20" s="9"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>21</v>
       </c>
@@ -2243,7 +2251,7 @@
       <c r="K21" s="11"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>22</v>
       </c>
@@ -2261,7 +2269,7 @@
       <c r="K22" s="11"/>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>23</v>
       </c>
@@ -2279,7 +2287,7 @@
       <c r="K23" s="11"/>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>24</v>
       </c>
@@ -2297,7 +2305,7 @@
       <c r="K24" s="11"/>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>25</v>
       </c>
@@ -2315,7 +2323,7 @@
       <c r="K25" s="11"/>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>26</v>
       </c>
@@ -2333,7 +2341,7 @@
       <c r="K26" s="11"/>
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>27</v>
       </c>
@@ -2351,7 +2359,7 @@
       <c r="K27" s="11"/>
       <c r="L27" s="9"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>28</v>
       </c>
@@ -2369,7 +2377,7 @@
       <c r="K28" s="11"/>
       <c r="L28" s="9"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>29</v>
       </c>
@@ -2387,7 +2395,7 @@
       <c r="K29" s="11"/>
       <c r="L29" s="9"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>30</v>
       </c>
@@ -2405,7 +2413,7 @@
       <c r="K30" s="11"/>
       <c r="L30" s="9"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>31</v>
       </c>
@@ -2423,7 +2431,7 @@
       <c r="K31" s="11"/>
       <c r="L31" s="9"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>32</v>
       </c>
@@ -2441,7 +2449,7 @@
       <c r="K32" s="11"/>
       <c r="L32" s="9"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>33</v>
       </c>
@@ -2459,7 +2467,7 @@
       <c r="K33" s="11"/>
       <c r="L33" s="9"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
@@ -2485,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="5" t="s">
@@ -2502,7 +2510,7 @@
       <c r="I35" s="4"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -2541,18 +2549,18 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
@@ -2572,7 +2580,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2592,7 +2600,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2612,7 +2620,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2632,7 +2640,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2652,7 +2660,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -2692,7 +2700,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2712,7 +2720,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2732,23 +2740,47 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2">
+        <v>44523</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>31100</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2">
+        <v>44241</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2756,7 +2788,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2764,7 +2796,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2772,7 +2804,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2780,7 +2812,7 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2788,7 +2820,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2796,7 +2828,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2804,7 +2836,7 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2812,7 +2844,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2820,7 +2852,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2828,7 +2860,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2836,7 +2868,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>

</xml_diff>